<commit_message>
Written ReadExcelCar (read excel file code) for CarInsurance. Updated Excel file InputData.xlsx file with CarInsurance Data. Data-Driven using Apache POI completed.
</commit_message>
<xml_diff>
--- a/src/main/resources/Inputdata.xlsx
+++ b/src/main/resources/Inputdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software testing\IntelliJ\5_6160956923404354197\StudentInsurance\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software testing\IntelliJ\5_6160956923404354197\StudentSubmission\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TravelInsurance" sheetId="1" r:id="rId1"/>
@@ -25,34 +25,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Age for Trav1</t>
-  </si>
-  <si>
-    <t>Age for Trav 2</t>
-  </si>
-  <si>
-    <t>Phone number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>France</t>
   </si>
   <si>
     <t>S.No</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>age1</t>
+  </si>
+  <si>
+    <t>age2</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>MP14</t>
+  </si>
+  <si>
+    <t>John Cenna</t>
+  </si>
+  <si>
+    <t>invalid email</t>
+  </si>
+  <si>
+    <t>valid email</t>
+  </si>
+  <si>
+    <t>john123</t>
+  </si>
+  <si>
+    <t>invalid phone</t>
+  </si>
+  <si>
+    <t>valid phone</t>
+  </si>
+  <si>
+    <t>john123@gmail.com</t>
+  </si>
+  <si>
+    <t>place</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -375,19 +417,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -395,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>21</v>
@@ -414,14 +456,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>987654321</v>
+      </c>
+      <c r="G2">
+        <v>9876543210</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Work on getTravelInsuranceData method for returning valid map for TravelInsuranceTests
</commit_message>
<xml_diff>
--- a/src/main/resources/Inputdata.xlsx
+++ b/src/main/resources/Inputdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software testing\IntelliJ\5_6160956923404354197\StudentSubmission\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prateek_parashar\code\Hackathon\StudentSubmission\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC8ACE0-6D2B-4242-AC98-39CBEBC8C4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190" activeTab="1"/>
+    <workbookView xWindow="-17580" yWindow="-270" windowWidth="14670" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TravelInsurance" sheetId="1" r:id="rId1"/>
@@ -42,9 +43,6 @@
     <t>age2</t>
   </si>
   <si>
-    <t>phonenumber</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -73,12 +71,15 @@
   </si>
   <si>
     <t>place</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,10 +118,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -401,21 +404,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -429,88 +432,89 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>21</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>22</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>9876543210</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>987654321</v>
@@ -521,7 +525,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Parallel execution of tests is working now. Cheers
</commit_message>
<xml_diff>
--- a/src/main/resources/Inputdata.xlsx
+++ b/src/main/resources/Inputdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prateek_parashar\code\Hackathon\StudentSubmission\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC8ACE0-6D2B-4242-AC98-39CBEBC8C4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494E48F4-4EE7-4E8C-8569-8B3F11536E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17580" yWindow="-270" windowWidth="14670" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17580" yWindow="-270" windowWidth="14670" windowHeight="8325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TravelInsurance" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>MP14</t>
   </si>
   <si>
-    <t>John Cenna</t>
-  </si>
-  <si>
     <t>invalid email</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>John Cena</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -432,7 +432,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,22 +481,22 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
       <c r="J1" s="1"/>
     </row>
@@ -508,13 +508,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>987654321</v>

</xml_diff>